<commit_message>
Upload Y4_B2526_Immuno&hema_scanner1757236162193_d00cfd5e70ceccca002dc2270b48d57750b4810fb0e2d7436582e39586577055.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_Immuno&hema_scanner1757236162193_d00cfd5e70ceccca002dc2270b48d57750b4810fb0e2d7436582e39586577055.xlsx
+++ b/log_history/Y4_B2526_Immuno&hema_scanner1757236162193_d00cfd5e70ceccca002dc2270b48d57750b4810fb0e2d7436582e39586577055.xlsx
@@ -1,41 +1,95 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\log_history\Imported_logs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A9B27A-5CD1-4518-9D32-DFC431700D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="1520" yWindow="1300" windowWidth="18280" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Scanner" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+  <si>
+    <t>Student ID</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Log Date</t>
+  </si>
+  <si>
+    <t>Log Time</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>221454</t>
+  </si>
+  <si>
+    <t>07/09/2025</t>
+  </si>
+  <si>
+    <t>11:09:37</t>
+  </si>
+  <si>
+    <t>Manual</t>
+  </si>
+  <si>
+    <t>160392@med.asu.edu.com</t>
+  </si>
+  <si>
+    <t>221469</t>
+  </si>
+  <si>
+    <t>11:32:31</t>
+  </si>
+  <si>
+    <t>Scan</t>
+  </si>
+  <si>
+    <t>221482</t>
+  </si>
+  <si>
+    <t>11:33:22</t>
+  </si>
+  <si>
+    <t>221586</t>
+  </si>
+  <si>
+    <t>11:33:43</t>
+  </si>
+  <si>
+    <t>221514</t>
+  </si>
+  <si>
+    <t>11:33:52</t>
+  </si>
+  <si>
+    <t>Immuno&amp;hema</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -43,13 +97,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF0F0F0"/>
+        <bgColor rgb="FFF0F0F0"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -64,14 +129,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,135 +472,142 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B6"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="24.4140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Student ID</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Subject</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Log Date</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Log Time</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Type</v>
-      </c>
-      <c r="F1" t="str">
-        <v>User</v>
+    <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>221454</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Internal Medicine 1</v>
-      </c>
-      <c r="C2" t="str">
-        <v>07/09/2025</v>
-      </c>
-      <c r="D2" t="str">
-        <v>11:09:37</v>
-      </c>
-      <c r="E2" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F2" t="str">
-        <v>160392@med.asu.edu.com</v>
+    <row r="2" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>221469</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Internal Medicine 1</v>
-      </c>
-      <c r="C3" t="str">
-        <v>07/09/2025</v>
-      </c>
-      <c r="D3" t="str">
-        <v>11:32:31</v>
-      </c>
-      <c r="E3" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F3" t="str">
-        <v>160392@med.asu.edu.com</v>
+    <row r="3" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>221482</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Internal Medicine 1</v>
-      </c>
-      <c r="C4" t="str">
-        <v>07/09/2025</v>
-      </c>
-      <c r="D4" t="str">
-        <v>11:33:22</v>
-      </c>
-      <c r="E4" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F4" t="str">
-        <v>160392@med.asu.edu.com</v>
+    <row r="4" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>221586</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Internal Medicine 1</v>
-      </c>
-      <c r="C5" t="str">
-        <v>07/09/2025</v>
-      </c>
-      <c r="D5" t="str">
-        <v>11:33:43</v>
-      </c>
-      <c r="E5" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F5" t="str">
-        <v>160392@med.asu.edu.com</v>
+    <row r="5" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>221514</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Internal Medicine 1</v>
-      </c>
-      <c r="C6" t="str">
-        <v>07/09/2025</v>
-      </c>
-      <c r="D6" t="str">
-        <v>11:33:52</v>
-      </c>
-      <c r="E6" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F6" t="str">
-        <v>160392@med.asu.edu.com</v>
+    <row r="6" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F6"/>
+    <ignoredError sqref="A1:F1 A3:A6 A2 C2:F2 C3:F6" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>